<commit_message>
thêm bảng sửa thông tin user
</commit_message>
<xml_diff>
--- a/reque/SMS_Gateway_Requirements_20171115.xlsx
+++ b/reque/SMS_Gateway_Requirements_20171115.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2429" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="836">
   <si>
     <t>No.</t>
   </si>
@@ -2228,13 +2228,7 @@
     <t>Chi phí cho 1 tin cài đặt theo từng admin hoặc customer</t>
   </si>
   <si>
-    <t>TABLE "Manager_Setting"</t>
-  </si>
-  <si>
     <t>TABLE "User_Carrier_Setting"</t>
-  </si>
-  <si>
-    <t>TABLE "Customer_Setting"</t>
   </si>
   <si>
     <t>- Thêm mới tài khoản quản lý (SuperAdmin, Admin, Customer)</t>
@@ -2697,6 +2691,15 @@
   </si>
   <si>
     <t>type = 2</t>
+  </si>
+  <si>
+    <t>TABLE "web_user_setting"</t>
+  </si>
+  <si>
+    <t>TABLE "Customer_Setting"=&gt;không dùng</t>
+  </si>
+  <si>
+    <t>TABLE "Manager_Setting"=&gt; không dùng</t>
   </si>
 </sst>
 </file>
@@ -18423,40 +18426,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="259" fillId="3" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="259" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="259" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="259" fillId="3" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="259" fillId="3" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="260" fillId="0" borderId="96" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="259" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="259" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="96" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="260" fillId="0" borderId="96" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="96" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="96" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -23845,7 +23848,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D1AB13FB-E9FE-4C12-86A9-7360E72E51C9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1AB13FB-E9FE-4C12-86A9-7360E72E51C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24183,25 +24186,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33.75" customHeight="1">
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="110" t="s">
         <v>483</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="114" t="s">
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="113" t="s">
         <v>477</v>
       </c>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114" t="s">
+      <c r="G1" s="113"/>
+      <c r="H1" s="113" t="s">
         <v>476</v>
       </c>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114" t="s">
+      <c r="I1" s="113"/>
+      <c r="J1" s="113" t="s">
         <v>601</v>
       </c>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114" t="s">
+      <c r="K1" s="113"/>
+      <c r="L1" s="113" t="s">
         <v>427</v>
       </c>
     </row>
@@ -24237,14 +24240,14 @@
       <c r="K2" s="37" t="s">
         <v>455</v>
       </c>
-      <c r="L2" s="114"/>
+      <c r="L2" s="113"/>
     </row>
     <row r="3" spans="1:12" s="10" customFormat="1">
       <c r="A3" s="7"/>
       <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="107" t="s">
         <v>590</v>
       </c>
       <c r="D3" s="73" t="s">
@@ -24276,9 +24279,9 @@
     <row r="4" spans="1:12" s="10" customFormat="1">
       <c r="A4" s="7"/>
       <c r="B4" s="46"/>
-      <c r="C4" s="109"/>
+      <c r="C4" s="108"/>
       <c r="D4" s="73" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E4" s="43">
         <v>0</v>
@@ -24306,9 +24309,9 @@
     <row r="5" spans="1:12" s="10" customFormat="1">
       <c r="A5" s="7"/>
       <c r="B5" s="46"/>
-      <c r="C5" s="110"/>
+      <c r="C5" s="109"/>
       <c r="D5" s="73" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E5" s="43">
         <v>0</v>
@@ -24336,7 +24339,7 @@
     <row r="6" spans="1:12" s="10" customFormat="1">
       <c r="A6" s="7"/>
       <c r="B6" s="46"/>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="107" t="s">
         <v>425</v>
       </c>
       <c r="D6" s="73" t="s">
@@ -24370,7 +24373,7 @@
       <c r="B7" s="41">
         <v>2</v>
       </c>
-      <c r="C7" s="109"/>
+      <c r="C7" s="108"/>
       <c r="D7" s="73" t="s">
         <v>706</v>
       </c>
@@ -24402,7 +24405,7 @@
       <c r="B8" s="41">
         <v>3</v>
       </c>
-      <c r="C8" s="110"/>
+      <c r="C8" s="109"/>
       <c r="D8" s="73" t="s">
         <v>707</v>
       </c>
@@ -24434,7 +24437,7 @@
       <c r="B9" s="41">
         <v>4</v>
       </c>
-      <c r="C9" s="107" t="s">
+      <c r="C9" s="114" t="s">
         <v>715</v>
       </c>
       <c r="D9" s="73" t="s">
@@ -24464,7 +24467,7 @@
       <c r="B10" s="41">
         <v>5</v>
       </c>
-      <c r="C10" s="107"/>
+      <c r="C10" s="114"/>
       <c r="D10" s="73" t="s">
         <v>709</v>
       </c>
@@ -24492,7 +24495,7 @@
       <c r="B11" s="41">
         <v>6</v>
       </c>
-      <c r="C11" s="107"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="73" t="s">
         <v>710</v>
       </c>
@@ -24550,11 +24553,11 @@
       <c r="B13" s="41">
         <v>8</v>
       </c>
-      <c r="C13" s="107" t="s">
-        <v>730</v>
+      <c r="C13" s="114" t="s">
+        <v>728</v>
       </c>
       <c r="D13" s="76" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="E13" s="39">
         <v>2</v>
@@ -24580,9 +24583,9 @@
       <c r="B14" s="41">
         <v>9</v>
       </c>
-      <c r="C14" s="107"/>
+      <c r="C14" s="114"/>
       <c r="D14" s="76" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E14" s="39">
         <v>2</v>
@@ -24608,9 +24611,9 @@
       <c r="B15" s="41">
         <v>10</v>
       </c>
-      <c r="C15" s="107"/>
+      <c r="C15" s="114"/>
       <c r="D15" s="76" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E15" s="39">
         <v>2</v>
@@ -24636,9 +24639,9 @@
       <c r="B16" s="41">
         <v>11</v>
       </c>
-      <c r="C16" s="107"/>
+      <c r="C16" s="114"/>
       <c r="D16" s="84" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E16" s="39">
         <v>2</v>
@@ -24664,9 +24667,9 @@
       <c r="B17" s="41">
         <v>12</v>
       </c>
-      <c r="C17" s="107"/>
+      <c r="C17" s="114"/>
       <c r="D17" s="84" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="E17" s="39">
         <v>2</v>
@@ -24692,11 +24695,11 @@
       <c r="B18" s="41">
         <v>13</v>
       </c>
-      <c r="C18" s="107" t="s">
-        <v>746</v>
+      <c r="C18" s="114" t="s">
+        <v>744</v>
       </c>
       <c r="D18" s="85" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E18" s="39">
         <v>3</v>
@@ -24722,9 +24725,9 @@
       <c r="B19" s="41">
         <v>14</v>
       </c>
-      <c r="C19" s="107"/>
+      <c r="C19" s="114"/>
       <c r="D19" s="84" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E19" s="39">
         <v>3</v>
@@ -24750,9 +24753,9 @@
       <c r="B20" s="41">
         <v>15</v>
       </c>
-      <c r="C20" s="107"/>
+      <c r="C20" s="114"/>
       <c r="D20" s="84" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E20" s="39">
         <v>3</v>
@@ -24777,11 +24780,11 @@
       <c r="B21" s="41">
         <v>16</v>
       </c>
-      <c r="C21" s="108" t="s">
-        <v>752</v>
+      <c r="C21" s="107" t="s">
+        <v>750</v>
       </c>
       <c r="D21" s="84" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E21" s="40">
         <v>4</v>
@@ -24806,9 +24809,9 @@
       <c r="B22" s="41">
         <v>17</v>
       </c>
-      <c r="C22" s="109"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="84" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E22" s="40">
         <v>4</v>
@@ -24833,9 +24836,9 @@
       <c r="B23" s="41">
         <v>18</v>
       </c>
-      <c r="C23" s="109"/>
+      <c r="C23" s="108"/>
       <c r="D23" s="84" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E23" s="40">
         <v>4</v>
@@ -24860,9 +24863,9 @@
       <c r="B24" s="41">
         <v>19</v>
       </c>
-      <c r="C24" s="109"/>
+      <c r="C24" s="108"/>
       <c r="D24" s="70" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="E24" s="40">
         <v>5</v>
@@ -24887,7 +24890,7 @@
       <c r="B25" s="41">
         <v>20</v>
       </c>
-      <c r="C25" s="109"/>
+      <c r="C25" s="108"/>
       <c r="D25" s="84" t="s">
         <v>612</v>
       </c>
@@ -24914,8 +24917,8 @@
       <c r="B26" s="41">
         <v>21</v>
       </c>
-      <c r="C26" s="108" t="s">
-        <v>822</v>
+      <c r="C26" s="107" t="s">
+        <v>820</v>
       </c>
       <c r="D26" s="84" t="s">
         <v>553</v>
@@ -24943,7 +24946,7 @@
       <c r="B27" s="41">
         <v>22</v>
       </c>
-      <c r="C27" s="109"/>
+      <c r="C27" s="108"/>
       <c r="D27" s="84" t="s">
         <v>554</v>
       </c>
@@ -24970,7 +24973,7 @@
       <c r="B28" s="41">
         <v>23</v>
       </c>
-      <c r="C28" s="109"/>
+      <c r="C28" s="108"/>
       <c r="D28" s="84" t="s">
         <v>555</v>
       </c>
@@ -24997,7 +25000,7 @@
       <c r="B29" s="41">
         <v>24</v>
       </c>
-      <c r="C29" s="109"/>
+      <c r="C29" s="108"/>
       <c r="D29" s="84" t="s">
         <v>556</v>
       </c>
@@ -25024,7 +25027,7 @@
       <c r="B30" s="41">
         <v>25</v>
       </c>
-      <c r="C30" s="109"/>
+      <c r="C30" s="108"/>
       <c r="D30" s="84" t="s">
         <v>557</v>
       </c>
@@ -25051,11 +25054,11 @@
       <c r="B31" s="41">
         <v>26</v>
       </c>
-      <c r="C31" s="107" t="s">
+      <c r="C31" s="114" t="s">
         <v>559</v>
       </c>
       <c r="D31" s="84" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="E31" s="40">
         <v>1</v>
@@ -25084,9 +25087,9 @@
       <c r="B32" s="41">
         <v>27</v>
       </c>
-      <c r="C32" s="107"/>
+      <c r="C32" s="114"/>
       <c r="D32" s="84" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E32" s="40">
         <v>1</v>
@@ -25111,11 +25114,11 @@
       <c r="B33" s="41">
         <v>28</v>
       </c>
-      <c r="C33" s="107" t="s">
+      <c r="C33" s="114" t="s">
         <v>481</v>
       </c>
       <c r="D33" s="76" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E33" s="40">
         <v>1</v>
@@ -25144,9 +25147,9 @@
       <c r="B34" s="41">
         <v>29</v>
       </c>
-      <c r="C34" s="107"/>
+      <c r="C34" s="114"/>
       <c r="D34" s="85" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E34" s="40">
         <v>2</v>
@@ -25171,9 +25174,9 @@
       <c r="B35" s="41">
         <v>30</v>
       </c>
-      <c r="C35" s="107"/>
+      <c r="C35" s="114"/>
       <c r="D35" s="85" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="E35" s="39">
         <v>3</v>
@@ -25198,9 +25201,9 @@
       <c r="B36" s="41">
         <v>31</v>
       </c>
-      <c r="C36" s="107"/>
+      <c r="C36" s="114"/>
       <c r="D36" s="85" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E36" s="39">
         <v>3</v>
@@ -25225,9 +25228,9 @@
       <c r="B37" s="41">
         <v>32</v>
       </c>
-      <c r="C37" s="107"/>
+      <c r="C37" s="114"/>
       <c r="D37" s="76" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E37" s="40">
         <v>4</v>
@@ -25252,9 +25255,9 @@
       <c r="B38" s="41">
         <v>33</v>
       </c>
-      <c r="C38" s="107"/>
+      <c r="C38" s="114"/>
       <c r="D38" s="85" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E38" s="40">
         <v>4</v>
@@ -25279,9 +25282,9 @@
       <c r="B39" s="41">
         <v>34</v>
       </c>
-      <c r="C39" s="107"/>
+      <c r="C39" s="114"/>
       <c r="D39" s="85" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E39" s="40">
         <v>4</v>
@@ -25306,7 +25309,7 @@
       <c r="B40" s="41">
         <v>35</v>
       </c>
-      <c r="C40" s="107"/>
+      <c r="C40" s="114"/>
       <c r="D40" s="76" t="s">
         <v>679</v>
       </c>
@@ -25333,7 +25336,7 @@
       <c r="B41" s="41">
         <v>36</v>
       </c>
-      <c r="C41" s="107"/>
+      <c r="C41" s="114"/>
       <c r="D41" s="85" t="s">
         <v>487</v>
       </c>
@@ -25387,8 +25390,8 @@
     </row>
     <row r="43" spans="2:12">
       <c r="B43" s="41"/>
-      <c r="C43" s="108" t="s">
-        <v>819</v>
+      <c r="C43" s="107" t="s">
+        <v>817</v>
       </c>
       <c r="D43" s="84" t="s">
         <v>600</v>
@@ -25414,7 +25417,7 @@
     </row>
     <row r="44" spans="2:12">
       <c r="B44" s="41"/>
-      <c r="C44" s="109"/>
+      <c r="C44" s="108"/>
       <c r="D44" s="84" t="s">
         <v>598</v>
       </c>
@@ -25439,7 +25442,7 @@
     </row>
     <row r="45" spans="2:12">
       <c r="B45" s="41"/>
-      <c r="C45" s="110"/>
+      <c r="C45" s="109"/>
       <c r="D45" s="84" t="s">
         <v>599</v>
       </c>
@@ -25464,12 +25467,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="C33:C41"/>
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="C9:C11"/>
@@ -25479,6 +25476,12 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="C26:C30"/>
     <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -25549,7 +25552,7 @@
       <c r="A2" s="74">
         <v>1</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="114" t="s">
         <v>425</v>
       </c>
       <c r="C2" s="73" t="s">
@@ -25561,7 +25564,7 @@
       <c r="E2" s="88">
         <v>0.5</v>
       </c>
-      <c r="F2" s="118" t="s">
+      <c r="F2" s="117" t="s">
         <v>714</v>
       </c>
       <c r="G2" s="92" t="s">
@@ -25579,7 +25582,7 @@
       <c r="A3" s="74">
         <v>2</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="114"/>
       <c r="C3" s="73" t="s">
         <v>706</v>
       </c>
@@ -25589,7 +25592,7 @@
       <c r="E3" s="88">
         <v>0.5</v>
       </c>
-      <c r="F3" s="118"/>
+      <c r="F3" s="117"/>
       <c r="G3" s="92" t="s">
         <v>569</v>
       </c>
@@ -25605,7 +25608,7 @@
       <c r="A4" s="74">
         <v>3</v>
       </c>
-      <c r="B4" s="107"/>
+      <c r="B4" s="114"/>
       <c r="C4" s="73" t="s">
         <v>707</v>
       </c>
@@ -25615,7 +25618,7 @@
       <c r="E4" s="88">
         <v>0</v>
       </c>
-      <c r="F4" s="118"/>
+      <c r="F4" s="117"/>
       <c r="G4" s="92" t="s">
         <v>569</v>
       </c>
@@ -25631,7 +25634,7 @@
       <c r="A5" s="74">
         <v>4</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="114" t="s">
         <v>715</v>
       </c>
       <c r="C5" s="73" t="s">
@@ -25657,7 +25660,7 @@
       <c r="A6" s="74">
         <v>5</v>
       </c>
-      <c r="B6" s="107"/>
+      <c r="B6" s="114"/>
       <c r="C6" s="73" t="s">
         <v>709</v>
       </c>
@@ -25679,7 +25682,7 @@
       <c r="A7" s="74">
         <v>6</v>
       </c>
-      <c r="B7" s="107"/>
+      <c r="B7" s="114"/>
       <c r="C7" s="73" t="s">
         <v>710</v>
       </c>
@@ -25701,10 +25704,10 @@
       <c r="A8" s="74">
         <v>7</v>
       </c>
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="114" t="s">
         <v>485</v>
       </c>
-      <c r="C8" s="117" t="s">
+      <c r="C8" s="118" t="s">
         <v>485</v>
       </c>
       <c r="D8" s="77" t="s">
@@ -25713,7 +25716,7 @@
       <c r="E8" s="89">
         <v>0.5</v>
       </c>
-      <c r="F8" s="117" t="s">
+      <c r="F8" s="118" t="s">
         <v>644</v>
       </c>
       <c r="G8" s="93" t="s">
@@ -25731,15 +25734,15 @@
       <c r="A9" s="74">
         <v>8</v>
       </c>
-      <c r="B9" s="107"/>
-      <c r="C9" s="117"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="118"/>
       <c r="D9" s="77" t="s">
         <v>562</v>
       </c>
       <c r="E9" s="89">
         <v>0.5</v>
       </c>
-      <c r="F9" s="117"/>
+      <c r="F9" s="118"/>
       <c r="G9" s="93" t="s">
         <v>569</v>
       </c>
@@ -25751,11 +25754,11 @@
       <c r="A10" s="74">
         <v>9</v>
       </c>
-      <c r="B10" s="107" t="s">
-        <v>730</v>
-      </c>
-      <c r="C10" s="117" t="s">
-        <v>735</v>
+      <c r="B10" s="114" t="s">
+        <v>728</v>
+      </c>
+      <c r="C10" s="118" t="s">
+        <v>733</v>
       </c>
       <c r="D10" s="84" t="s">
         <v>607</v>
@@ -25763,7 +25766,7 @@
       <c r="E10" s="87">
         <v>0.2</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F10" s="118" t="s">
         <v>644</v>
       </c>
       <c r="G10" s="93" t="s">
@@ -25777,15 +25780,15 @@
       <c r="A11" s="74">
         <v>10</v>
       </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="117"/>
+      <c r="B11" s="114"/>
+      <c r="C11" s="118"/>
       <c r="D11" s="79" t="s">
         <v>641</v>
       </c>
       <c r="E11" s="87">
         <v>0.5</v>
       </c>
-      <c r="F11" s="117"/>
+      <c r="F11" s="118"/>
       <c r="G11" s="93" t="s">
         <v>569</v>
       </c>
@@ -25797,15 +25800,15 @@
       <c r="A12" s="74">
         <v>11</v>
       </c>
-      <c r="B12" s="107"/>
-      <c r="C12" s="117"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="118"/>
       <c r="D12" s="79" t="s">
         <v>651</v>
       </c>
       <c r="E12" s="87">
         <v>0.2</v>
       </c>
-      <c r="F12" s="117"/>
+      <c r="F12" s="118"/>
       <c r="G12" s="93" t="s">
         <v>569</v>
       </c>
@@ -25817,12 +25820,12 @@
       <c r="A13" s="74">
         <v>12</v>
       </c>
-      <c r="B13" s="107"/>
+      <c r="B13" s="114"/>
       <c r="C13" s="76" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D13" s="84" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E13" s="87">
         <v>1</v>
@@ -25841,17 +25844,17 @@
       <c r="A14" s="74">
         <v>13</v>
       </c>
-      <c r="B14" s="107"/>
-      <c r="C14" s="117" t="s">
-        <v>732</v>
+      <c r="B14" s="114"/>
+      <c r="C14" s="118" t="s">
+        <v>730</v>
       </c>
       <c r="D14" s="77" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E14" s="89">
         <v>0.5</v>
       </c>
-      <c r="F14" s="117" t="s">
+      <c r="F14" s="118" t="s">
         <v>594</v>
       </c>
       <c r="G14" s="93" t="s">
@@ -25865,15 +25868,15 @@
       <c r="A15" s="74">
         <v>14</v>
       </c>
-      <c r="B15" s="107"/>
-      <c r="C15" s="117"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="118"/>
       <c r="D15" s="77" t="s">
         <v>560</v>
       </c>
       <c r="E15" s="89">
         <v>0.5</v>
       </c>
-      <c r="F15" s="117"/>
+      <c r="F15" s="118"/>
       <c r="G15" s="93" t="s">
         <v>569</v>
       </c>
@@ -25885,15 +25888,15 @@
       <c r="A16" s="74">
         <v>15</v>
       </c>
-      <c r="B16" s="107"/>
-      <c r="C16" s="117"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="77" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E16" s="89">
         <v>0.5</v>
       </c>
-      <c r="F16" s="117"/>
+      <c r="F16" s="118"/>
       <c r="G16" s="93" t="s">
         <v>569</v>
       </c>
@@ -25905,15 +25908,15 @@
       <c r="A17" s="74">
         <v>16</v>
       </c>
-      <c r="B17" s="107"/>
-      <c r="C17" s="117"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="118"/>
       <c r="D17" s="77" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E17" s="89">
         <v>0.5</v>
       </c>
-      <c r="F17" s="117"/>
+      <c r="F17" s="118"/>
       <c r="G17" s="93" t="s">
         <v>569</v>
       </c>
@@ -25925,18 +25928,18 @@
       <c r="A18" s="74">
         <v>17</v>
       </c>
-      <c r="B18" s="107"/>
-      <c r="C18" s="115" t="s">
-        <v>733</v>
+      <c r="B18" s="114"/>
+      <c r="C18" s="116" t="s">
+        <v>731</v>
       </c>
       <c r="D18" s="77" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E18" s="89">
         <v>1.5</v>
       </c>
       <c r="F18" s="80" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G18" s="93" t="s">
         <v>569</v>
@@ -25949,16 +25952,16 @@
       <c r="A19" s="74">
         <v>18</v>
       </c>
-      <c r="B19" s="107"/>
-      <c r="C19" s="115"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="116"/>
       <c r="D19" s="77" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E19" s="89">
         <v>1.5</v>
       </c>
       <c r="F19" s="80" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G19" s="93" t="s">
         <v>569</v>
@@ -25971,18 +25974,18 @@
       <c r="A20" s="74">
         <v>19</v>
       </c>
-      <c r="B20" s="107"/>
-      <c r="C20" s="115" t="s">
-        <v>734</v>
+      <c r="B20" s="114"/>
+      <c r="C20" s="116" t="s">
+        <v>732</v>
       </c>
       <c r="D20" s="77" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E20" s="89">
         <v>1.5</v>
       </c>
       <c r="F20" s="80" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G20" s="93" t="s">
         <v>569</v>
@@ -25995,16 +25998,16 @@
       <c r="A21" s="74">
         <v>20</v>
       </c>
-      <c r="B21" s="107"/>
-      <c r="C21" s="115"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="116"/>
       <c r="D21" s="77" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E21" s="89">
         <v>1.5</v>
       </c>
       <c r="F21" s="80" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G21" s="93" t="s">
         <v>569</v>
@@ -26017,20 +26020,20 @@
       <c r="A22" s="74">
         <v>21</v>
       </c>
-      <c r="B22" s="107" t="s">
-        <v>746</v>
+      <c r="B22" s="114" t="s">
+        <v>744</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E22" s="87">
         <v>0.5</v>
       </c>
       <c r="F22" s="83" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G22" s="92"/>
       <c r="H22" s="92" t="s">
@@ -26043,9 +26046,9 @@
       <c r="A23" s="74">
         <v>22</v>
       </c>
-      <c r="B23" s="107"/>
+      <c r="B23" s="114"/>
       <c r="C23" s="84" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D23" s="82" t="s">
         <v>623</v>
@@ -26067,9 +26070,9 @@
       <c r="A24" s="74">
         <v>23</v>
       </c>
-      <c r="B24" s="107"/>
-      <c r="C24" s="115" t="s">
-        <v>749</v>
+      <c r="B24" s="114"/>
+      <c r="C24" s="116" t="s">
+        <v>747</v>
       </c>
       <c r="D24" s="82" t="s">
         <v>621</v>
@@ -26077,7 +26080,7 @@
       <c r="E24" s="87">
         <v>1</v>
       </c>
-      <c r="F24" s="116" t="s">
+      <c r="F24" s="115" t="s">
         <v>704</v>
       </c>
       <c r="G24" s="93" t="s">
@@ -26093,15 +26096,15 @@
       <c r="A25" s="74">
         <v>24</v>
       </c>
-      <c r="B25" s="107"/>
-      <c r="C25" s="115"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="116"/>
       <c r="D25" s="82" t="s">
         <v>622</v>
       </c>
       <c r="E25" s="87">
         <v>2</v>
       </c>
-      <c r="F25" s="116"/>
+      <c r="F25" s="115"/>
       <c r="G25" s="93" t="s">
         <v>569</v>
       </c>
@@ -26115,11 +26118,11 @@
       <c r="A26" s="74">
         <v>25</v>
       </c>
-      <c r="B26" s="108" t="s">
-        <v>752</v>
-      </c>
-      <c r="C26" s="115" t="s">
+      <c r="B26" s="107" t="s">
         <v>750</v>
+      </c>
+      <c r="C26" s="116" t="s">
+        <v>748</v>
       </c>
       <c r="D26" s="77" t="s">
         <v>620</v>
@@ -26127,8 +26130,8 @@
       <c r="E26" s="89">
         <v>0.5</v>
       </c>
-      <c r="F26" s="116" t="s">
-        <v>791</v>
+      <c r="F26" s="115" t="s">
+        <v>789</v>
       </c>
       <c r="G26" s="93" t="s">
         <v>569</v>
@@ -26141,15 +26144,15 @@
       <c r="A27" s="74">
         <v>26</v>
       </c>
-      <c r="B27" s="109"/>
-      <c r="C27" s="115"/>
+      <c r="B27" s="108"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="77" t="s">
         <v>619</v>
       </c>
       <c r="E27" s="89">
         <v>1.5</v>
       </c>
-      <c r="F27" s="116"/>
+      <c r="F27" s="115"/>
       <c r="G27" s="93" t="s">
         <v>569</v>
       </c>
@@ -26161,15 +26164,15 @@
       <c r="A28" s="74">
         <v>27</v>
       </c>
-      <c r="B28" s="109"/>
-      <c r="C28" s="115"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="116"/>
       <c r="D28" s="77" t="s">
         <v>699</v>
       </c>
       <c r="E28" s="89">
         <v>3</v>
       </c>
-      <c r="F28" s="116"/>
+      <c r="F28" s="115"/>
       <c r="G28" s="93" t="s">
         <v>569</v>
       </c>
@@ -26181,9 +26184,9 @@
       <c r="A29" s="74">
         <v>28</v>
       </c>
-      <c r="B29" s="109"/>
-      <c r="C29" s="115" t="s">
-        <v>751</v>
+      <c r="B29" s="108"/>
+      <c r="C29" s="116" t="s">
+        <v>749</v>
       </c>
       <c r="D29" s="77" t="s">
         <v>624</v>
@@ -26191,8 +26194,8 @@
       <c r="E29" s="89">
         <v>0.5</v>
       </c>
-      <c r="F29" s="116" t="s">
-        <v>792</v>
+      <c r="F29" s="115" t="s">
+        <v>790</v>
       </c>
       <c r="G29" s="93"/>
       <c r="H29" s="93" t="s">
@@ -26205,15 +26208,15 @@
       <c r="A30" s="74">
         <v>29</v>
       </c>
-      <c r="B30" s="109"/>
-      <c r="C30" s="115"/>
+      <c r="B30" s="108"/>
+      <c r="C30" s="116"/>
       <c r="D30" s="77" t="s">
         <v>627</v>
       </c>
       <c r="E30" s="89">
         <v>1.5</v>
       </c>
-      <c r="F30" s="116"/>
+      <c r="F30" s="115"/>
       <c r="G30" s="93"/>
       <c r="H30" s="93" t="s">
         <v>569</v>
@@ -26225,15 +26228,15 @@
       <c r="A31" s="74">
         <v>30</v>
       </c>
-      <c r="B31" s="109"/>
-      <c r="C31" s="115"/>
+      <c r="B31" s="108"/>
+      <c r="C31" s="116"/>
       <c r="D31" s="77" t="s">
         <v>700</v>
       </c>
       <c r="E31" s="89">
         <v>3</v>
       </c>
-      <c r="F31" s="116"/>
+      <c r="F31" s="115"/>
       <c r="G31" s="93"/>
       <c r="H31" s="93" t="s">
         <v>569</v>
@@ -26245,18 +26248,18 @@
       <c r="A32" s="74">
         <v>31</v>
       </c>
-      <c r="B32" s="109"/>
-      <c r="C32" s="115" t="s">
+      <c r="B32" s="108"/>
+      <c r="C32" s="116" t="s">
+        <v>751</v>
+      </c>
+      <c r="D32" s="82" t="s">
         <v>753</v>
-      </c>
-      <c r="D32" s="82" t="s">
-        <v>755</v>
       </c>
       <c r="E32" s="87">
         <v>2</v>
       </c>
-      <c r="F32" s="116" t="s">
-        <v>791</v>
+      <c r="F32" s="115" t="s">
+        <v>789</v>
       </c>
       <c r="G32" s="93" t="s">
         <v>569</v>
@@ -26271,15 +26274,15 @@
       <c r="A33" s="74">
         <v>32</v>
       </c>
-      <c r="B33" s="109"/>
-      <c r="C33" s="115"/>
+      <c r="B33" s="108"/>
+      <c r="C33" s="116"/>
       <c r="D33" s="82" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E33" s="87">
         <v>0.5</v>
       </c>
-      <c r="F33" s="116"/>
+      <c r="F33" s="115"/>
       <c r="G33" s="93" t="s">
         <v>569</v>
       </c>
@@ -26293,9 +26296,9 @@
       <c r="A34" s="74">
         <v>33</v>
       </c>
-      <c r="B34" s="109"/>
+      <c r="B34" s="108"/>
       <c r="C34" s="71" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D34" s="60" t="s">
         <v>647</v>
@@ -26303,7 +26306,7 @@
       <c r="E34" s="91">
         <v>5</v>
       </c>
-      <c r="F34" s="116"/>
+      <c r="F34" s="115"/>
       <c r="G34" s="93"/>
       <c r="H34" s="92"/>
       <c r="I34" s="92"/>
@@ -26315,8 +26318,8 @@
       <c r="A35" s="74">
         <v>34</v>
       </c>
-      <c r="B35" s="109"/>
-      <c r="C35" s="115" t="s">
+      <c r="B35" s="108"/>
+      <c r="C35" s="116" t="s">
         <v>612</v>
       </c>
       <c r="D35" s="82" t="s">
@@ -26325,8 +26328,8 @@
       <c r="E35" s="87">
         <v>0.5</v>
       </c>
-      <c r="F35" s="116" t="s">
-        <v>793</v>
+      <c r="F35" s="115" t="s">
+        <v>791</v>
       </c>
       <c r="G35" s="93" t="s">
         <v>569</v>
@@ -26341,15 +26344,15 @@
       <c r="A36" s="74">
         <v>35</v>
       </c>
-      <c r="B36" s="109"/>
-      <c r="C36" s="115"/>
+      <c r="B36" s="108"/>
+      <c r="C36" s="116"/>
       <c r="D36" s="82" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E36" s="87">
         <v>2</v>
       </c>
-      <c r="F36" s="116"/>
+      <c r="F36" s="115"/>
       <c r="G36" s="93" t="s">
         <v>569</v>
       </c>
@@ -26363,16 +26366,16 @@
       <c r="A37" s="74">
         <v>36</v>
       </c>
-      <c r="B37" s="110"/>
-      <c r="C37" s="115"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="116"/>
       <c r="D37" s="82" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E37" s="87">
         <v>2</v>
       </c>
       <c r="F37" s="80" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G37" s="93" t="s">
         <v>569</v>
@@ -26387,20 +26390,20 @@
       <c r="A38" s="74">
         <v>37</v>
       </c>
-      <c r="B38" s="108" t="s">
-        <v>822</v>
-      </c>
-      <c r="C38" s="115" t="s">
+      <c r="B38" s="107" t="s">
+        <v>820</v>
+      </c>
+      <c r="C38" s="116" t="s">
         <v>553</v>
       </c>
       <c r="D38" s="82" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E38" s="87">
         <v>0.5</v>
       </c>
-      <c r="F38" s="116" t="s">
-        <v>763</v>
+      <c r="F38" s="115" t="s">
+        <v>761</v>
       </c>
       <c r="G38" s="93" t="s">
         <v>569</v>
@@ -26415,15 +26418,15 @@
       <c r="A39" s="74">
         <v>38</v>
       </c>
-      <c r="B39" s="109"/>
-      <c r="C39" s="115"/>
+      <c r="B39" s="108"/>
+      <c r="C39" s="116"/>
       <c r="D39" s="82" t="s">
         <v>565</v>
       </c>
       <c r="E39" s="87">
         <v>2</v>
       </c>
-      <c r="F39" s="116"/>
+      <c r="F39" s="115"/>
       <c r="G39" s="93" t="s">
         <v>569</v>
       </c>
@@ -26437,18 +26440,18 @@
       <c r="A40" s="74">
         <v>39</v>
       </c>
-      <c r="B40" s="109"/>
-      <c r="C40" s="115" t="s">
+      <c r="B40" s="108"/>
+      <c r="C40" s="116" t="s">
         <v>554</v>
       </c>
       <c r="D40" s="82" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E40" s="87">
         <v>0.5</v>
       </c>
       <c r="F40" s="83" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="G40" s="93" t="s">
         <v>569</v>
@@ -26463,16 +26466,16 @@
       <c r="A41" s="74">
         <v>40</v>
       </c>
-      <c r="B41" s="109"/>
-      <c r="C41" s="115"/>
+      <c r="B41" s="108"/>
+      <c r="C41" s="116"/>
       <c r="D41" s="82" t="s">
         <v>566</v>
       </c>
       <c r="E41" s="87">
         <v>1</v>
       </c>
-      <c r="F41" s="116" t="s">
-        <v>763</v>
+      <c r="F41" s="115" t="s">
+        <v>761</v>
       </c>
       <c r="G41" s="93" t="s">
         <v>569</v>
@@ -26487,17 +26490,17 @@
       <c r="A42" s="74">
         <v>41</v>
       </c>
-      <c r="B42" s="109"/>
-      <c r="C42" s="115" t="s">
+      <c r="B42" s="108"/>
+      <c r="C42" s="116" t="s">
         <v>555</v>
       </c>
       <c r="D42" s="82" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E42" s="87">
         <v>0.5</v>
       </c>
-      <c r="F42" s="116"/>
+      <c r="F42" s="115"/>
       <c r="G42" s="93" t="s">
         <v>569</v>
       </c>
@@ -26511,8 +26514,8 @@
       <c r="A43" s="74">
         <v>42</v>
       </c>
-      <c r="B43" s="109"/>
-      <c r="C43" s="115"/>
+      <c r="B43" s="108"/>
+      <c r="C43" s="116"/>
       <c r="D43" s="82" t="s">
         <v>567</v>
       </c>
@@ -26533,18 +26536,18 @@
       <c r="A44" s="74">
         <v>43</v>
       </c>
-      <c r="B44" s="109"/>
-      <c r="C44" s="115" t="s">
+      <c r="B44" s="108"/>
+      <c r="C44" s="116" t="s">
         <v>556</v>
       </c>
       <c r="D44" s="82" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E44" s="87">
         <v>0.5</v>
       </c>
-      <c r="F44" s="116" t="s">
-        <v>763</v>
+      <c r="F44" s="115" t="s">
+        <v>761</v>
       </c>
       <c r="G44" s="93" t="s">
         <v>569</v>
@@ -26559,15 +26562,15 @@
       <c r="A45" s="74">
         <v>44</v>
       </c>
-      <c r="B45" s="109"/>
-      <c r="C45" s="115"/>
+      <c r="B45" s="108"/>
+      <c r="C45" s="116"/>
       <c r="D45" s="82" t="s">
         <v>568</v>
       </c>
       <c r="E45" s="87">
         <v>1</v>
       </c>
-      <c r="F45" s="116"/>
+      <c r="F45" s="115"/>
       <c r="G45" s="93" t="s">
         <v>569</v>
       </c>
@@ -26581,8 +26584,8 @@
       <c r="A46" s="74">
         <v>45</v>
       </c>
-      <c r="B46" s="109"/>
-      <c r="C46" s="115" t="s">
+      <c r="B46" s="108"/>
+      <c r="C46" s="116" t="s">
         <v>557</v>
       </c>
       <c r="D46" s="82" t="s">
@@ -26591,8 +26594,8 @@
       <c r="E46" s="87">
         <v>0.5</v>
       </c>
-      <c r="F46" s="116" t="s">
-        <v>763</v>
+      <c r="F46" s="115" t="s">
+        <v>761</v>
       </c>
       <c r="G46" s="93" t="s">
         <v>569</v>
@@ -26607,15 +26610,15 @@
       <c r="A47" s="74">
         <v>46</v>
       </c>
-      <c r="B47" s="109"/>
-      <c r="C47" s="115"/>
+      <c r="B47" s="108"/>
+      <c r="C47" s="116"/>
       <c r="D47" s="82" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E47" s="87">
         <v>0.5</v>
       </c>
-      <c r="F47" s="116"/>
+      <c r="F47" s="115"/>
       <c r="G47" s="93" t="s">
         <v>569</v>
       </c>
@@ -26629,15 +26632,15 @@
       <c r="A48" s="74">
         <v>47</v>
       </c>
-      <c r="B48" s="110"/>
-      <c r="C48" s="115"/>
+      <c r="B48" s="109"/>
+      <c r="C48" s="116"/>
       <c r="D48" s="82" t="s">
         <v>558</v>
       </c>
       <c r="E48" s="87">
         <v>1</v>
       </c>
-      <c r="F48" s="116"/>
+      <c r="F48" s="115"/>
       <c r="G48" s="93" t="s">
         <v>569</v>
       </c>
@@ -26651,19 +26654,19 @@
       <c r="A49" s="74">
         <v>48</v>
       </c>
-      <c r="B49" s="107" t="s">
+      <c r="B49" s="114" t="s">
         <v>559</v>
       </c>
-      <c r="C49" s="115" t="s">
+      <c r="C49" s="116" t="s">
+        <v>762</v>
+      </c>
+      <c r="D49" s="82" t="s">
         <v>764</v>
-      </c>
-      <c r="D49" s="82" t="s">
-        <v>766</v>
       </c>
       <c r="E49" s="87">
         <v>0.2</v>
       </c>
-      <c r="F49" s="116" t="s">
+      <c r="F49" s="115" t="s">
         <v>644</v>
       </c>
       <c r="G49" s="93" t="s">
@@ -26679,15 +26682,15 @@
       <c r="A50" s="74">
         <v>49</v>
       </c>
-      <c r="B50" s="107"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="114"/>
+      <c r="C50" s="116"/>
       <c r="D50" s="82" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="E50" s="87">
         <v>0.2</v>
       </c>
-      <c r="F50" s="116"/>
+      <c r="F50" s="115"/>
       <c r="G50" s="93" t="s">
         <v>569</v>
       </c>
@@ -26699,17 +26702,17 @@
       <c r="A51" s="74">
         <v>50</v>
       </c>
-      <c r="B51" s="107"/>
-      <c r="C51" s="115" t="s">
-        <v>765</v>
+      <c r="B51" s="114"/>
+      <c r="C51" s="116" t="s">
+        <v>763</v>
       </c>
       <c r="D51" s="82" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E51" s="87">
         <v>0.2</v>
       </c>
-      <c r="F51" s="116"/>
+      <c r="F51" s="115"/>
       <c r="G51" s="93" t="s">
         <v>569</v>
       </c>
@@ -26723,15 +26726,15 @@
       <c r="A52" s="74">
         <v>51</v>
       </c>
-      <c r="B52" s="107"/>
-      <c r="C52" s="115"/>
+      <c r="B52" s="114"/>
+      <c r="C52" s="116"/>
       <c r="D52" s="82" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="E52" s="87">
         <v>0.2</v>
       </c>
-      <c r="F52" s="116"/>
+      <c r="F52" s="115"/>
       <c r="G52" s="93" t="s">
         <v>569</v>
       </c>
@@ -26743,11 +26746,11 @@
       <c r="A53" s="74">
         <v>52</v>
       </c>
-      <c r="B53" s="107" t="s">
+      <c r="B53" s="114" t="s">
         <v>481</v>
       </c>
       <c r="C53" s="76" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D53" s="77" t="s">
         <v>606</v>
@@ -26774,9 +26777,9 @@
       <c r="A54" s="74">
         <v>53</v>
       </c>
-      <c r="B54" s="107"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="85" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D54" s="77" t="s">
         <v>486</v>
@@ -26800,18 +26803,18 @@
       <c r="A55" s="74">
         <v>54</v>
       </c>
-      <c r="B55" s="107"/>
+      <c r="B55" s="114"/>
       <c r="C55" s="85" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D55" s="77" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E55" s="89">
         <v>2</v>
       </c>
       <c r="F55" s="85" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G55" s="93"/>
       <c r="H55" s="93"/>
@@ -26824,12 +26827,12 @@
       <c r="A56" s="74">
         <v>55</v>
       </c>
-      <c r="B56" s="107"/>
+      <c r="B56" s="114"/>
       <c r="C56" s="85" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D56" s="77" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="E56" s="89">
         <v>1</v>
@@ -26848,18 +26851,18 @@
       <c r="A57" s="74">
         <v>56</v>
       </c>
-      <c r="B57" s="107"/>
-      <c r="C57" s="117" t="s">
-        <v>811</v>
+      <c r="B57" s="114"/>
+      <c r="C57" s="118" t="s">
+        <v>809</v>
       </c>
       <c r="D57" s="77" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E57" s="89">
         <v>1</v>
       </c>
       <c r="F57" s="85" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="G57" s="93"/>
       <c r="H57" s="93" t="s">
@@ -26872,16 +26875,16 @@
       <c r="A58" s="74">
         <v>57</v>
       </c>
-      <c r="B58" s="107"/>
-      <c r="C58" s="117"/>
+      <c r="B58" s="114"/>
+      <c r="C58" s="118"/>
       <c r="D58" s="77" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E58" s="89">
         <v>3</v>
       </c>
       <c r="F58" s="85" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="G58" s="93"/>
       <c r="H58" s="93"/>
@@ -26894,18 +26897,18 @@
       <c r="A59" s="74">
         <v>58</v>
       </c>
-      <c r="B59" s="107"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="85" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D59" s="77" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E59" s="89">
         <v>2</v>
       </c>
       <c r="F59" s="85" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G59" s="93"/>
       <c r="H59" s="93"/>
@@ -26918,18 +26921,18 @@
       <c r="A60" s="74">
         <v>59</v>
       </c>
-      <c r="B60" s="107"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="85" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D60" s="77" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E60" s="89">
         <v>2</v>
       </c>
       <c r="F60" s="85" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="G60" s="93"/>
       <c r="H60" s="93"/>
@@ -26942,7 +26945,7 @@
       <c r="A61" s="74">
         <v>60</v>
       </c>
-      <c r="B61" s="107"/>
+      <c r="B61" s="114"/>
       <c r="C61" s="76" t="s">
         <v>679</v>
       </c>
@@ -26964,12 +26967,12 @@
       <c r="A62" s="74">
         <v>61</v>
       </c>
-      <c r="B62" s="107"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="85" t="s">
         <v>487</v>
       </c>
       <c r="D62" s="77" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="E62" s="89">
         <v>2</v>
@@ -26990,10 +26993,10 @@
       <c r="A63" s="74">
         <v>62</v>
       </c>
-      <c r="B63" s="107" t="s">
+      <c r="B63" s="114" t="s">
         <v>482</v>
       </c>
-      <c r="C63" s="115" t="s">
+      <c r="C63" s="116" t="s">
         <v>597</v>
       </c>
       <c r="D63" s="82" t="s">
@@ -27014,8 +27017,8 @@
       <c r="A64" s="74">
         <v>63</v>
       </c>
-      <c r="B64" s="107"/>
-      <c r="C64" s="115"/>
+      <c r="B64" s="114"/>
+      <c r="C64" s="116"/>
       <c r="D64" s="82" t="s">
         <v>655</v>
       </c>
@@ -27034,8 +27037,8 @@
       <c r="A65" s="74">
         <v>64</v>
       </c>
-      <c r="B65" s="107"/>
-      <c r="C65" s="115"/>
+      <c r="B65" s="114"/>
+      <c r="C65" s="116"/>
       <c r="D65" s="82" t="s">
         <v>654</v>
       </c>
@@ -27052,14 +27055,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="B26:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C63:C65"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="B38:B48"/>
+    <mergeCell ref="B53:B62"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="F49:F52"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="F29:F31"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="F2:F4"/>
@@ -27074,28 +27091,14 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="C63:C65"/>
-    <mergeCell ref="B63:B65"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="B38:B48"/>
-    <mergeCell ref="B53:B62"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="F49:F52"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="B26:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C38:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -27104,10 +27107,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G216"/>
+  <dimension ref="A1:G238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -27591,7 +27594,7 @@
         <v>639</v>
       </c>
       <c r="G29" s="56" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -27612,7 +27615,7 @@
         <v>694</v>
       </c>
       <c r="G30" s="56" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -27633,7 +27636,7 @@
         <v>604</v>
       </c>
       <c r="G31" s="56" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -27654,7 +27657,7 @@
         <v>693</v>
       </c>
       <c r="G32" s="56" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -27944,7 +27947,7 @@
     </row>
     <row r="52" spans="1:6" s="11" customFormat="1">
       <c r="A52" s="104" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D52" s="105"/>
       <c r="F52" s="106"/>
@@ -28187,7 +28190,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:7">
       <c r="A65" s="98">
         <v>10</v>
       </c>
@@ -28207,7 +28210,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:7">
       <c r="A66" s="95">
         <v>11</v>
       </c>
@@ -28227,7 +28230,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:7">
       <c r="A67" s="98">
         <v>12</v>
       </c>
@@ -28247,7 +28250,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:7">
       <c r="A68" s="98">
         <v>18</v>
       </c>
@@ -28265,7 +28268,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:7">
       <c r="A69" s="95">
         <v>19</v>
       </c>
@@ -28283,47 +28286,62 @@
         <v>439</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:7">
       <c r="A70" s="57" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="56"/>
-      <c r="D71" s="56"/>
-      <c r="F71" s="56"/>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="104" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="53" t="s">
+    <row r="71" spans="1:7">
+      <c r="A71" s="104" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="53" t="s">
+      <c r="B72" s="53" t="s">
         <v>429</v>
       </c>
-      <c r="C73" s="53" t="s">
+      <c r="C72" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="D73" s="53" t="s">
+      <c r="D72" s="53" t="s">
         <v>496</v>
       </c>
-      <c r="E73" s="54" t="s">
+      <c r="E72" s="54" t="s">
         <v>431</v>
       </c>
-      <c r="F73" s="55" t="s">
+      <c r="F72" s="55" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="95">
+    <row r="73" spans="1:7">
+      <c r="A73" s="95">
         <v>1</v>
       </c>
-      <c r="B74" s="96" t="s">
+      <c r="B73" s="96" t="s">
         <v>432</v>
+      </c>
+      <c r="C73" s="96" t="s">
+        <v>434</v>
+      </c>
+      <c r="D73" s="97">
+        <v>8</v>
+      </c>
+      <c r="E73" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F73" s="78" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="64">
+        <v>2</v>
+      </c>
+      <c r="B74" s="102" t="s">
+        <v>827</v>
       </c>
       <c r="C74" s="96" t="s">
         <v>434</v>
@@ -28335,75 +28353,75 @@
         <v>435</v>
       </c>
       <c r="F74" s="78" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="64">
         <v>2</v>
       </c>
       <c r="B75" s="102" t="s">
-        <v>829</v>
-      </c>
-      <c r="C75" s="96" t="s">
-        <v>434</v>
-      </c>
-      <c r="D75" s="97">
-        <v>8</v>
+        <v>584</v>
+      </c>
+      <c r="C75" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="D75" s="100">
+        <v>200</v>
       </c>
       <c r="E75" s="96" t="s">
-        <v>435</v>
-      </c>
-      <c r="F75" s="78" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>452</v>
+      </c>
+      <c r="F75" s="79" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="64">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B76" s="102" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C76" s="99" t="s">
         <v>488</v>
       </c>
       <c r="D76" s="100">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="E76" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F76" s="79" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="64">
+        <v>4</v>
+      </c>
+      <c r="B77" s="99" t="s">
+        <v>552</v>
+      </c>
+      <c r="C77" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D77" s="100">
+        <v>2</v>
+      </c>
+      <c r="E77" s="96" t="s">
         <v>452</v>
       </c>
-      <c r="F76" s="79" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="64">
-        <v>3</v>
-      </c>
-      <c r="B77" s="102" t="s">
-        <v>585</v>
-      </c>
-      <c r="C77" s="99" t="s">
-        <v>488</v>
-      </c>
-      <c r="D77" s="100">
-        <v>50</v>
-      </c>
-      <c r="E77" s="96" t="s">
-        <v>435</v>
-      </c>
-      <c r="F77" s="79" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="64">
-        <v>4</v>
-      </c>
-      <c r="B78" s="99" t="s">
-        <v>552</v>
+      <c r="F77" s="101" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="95">
+        <v>5</v>
+      </c>
+      <c r="B78" s="102" t="s">
+        <v>587</v>
       </c>
       <c r="C78" s="99" t="s">
         <v>438</v>
@@ -28414,56 +28432,59 @@
       <c r="E78" s="96" t="s">
         <v>452</v>
       </c>
-      <c r="F78" s="101" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="95">
-        <v>5</v>
-      </c>
-      <c r="B79" s="102" t="s">
-        <v>587</v>
+      <c r="F78" s="79" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="64">
+        <v>6</v>
+      </c>
+      <c r="B79" s="99" t="s">
+        <v>547</v>
       </c>
       <c r="C79" s="99" t="s">
-        <v>438</v>
+        <v>549</v>
       </c>
       <c r="D79" s="100">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E79" s="96" t="s">
         <v>452</v>
       </c>
-      <c r="F79" s="79" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="64">
+      <c r="F79" s="101" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="95">
+        <v>7</v>
+      </c>
+      <c r="B80" s="99" t="s">
+        <v>499</v>
+      </c>
+      <c r="C80" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D80" s="100">
+        <v>2</v>
+      </c>
+      <c r="E80" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F80" s="101" t="s">
+        <v>500</v>
+      </c>
+      <c r="G80" s="56" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="31.5">
+      <c r="A81" s="64">
         <v>6</v>
       </c>
-      <c r="B80" s="99" t="s">
-        <v>547</v>
-      </c>
-      <c r="C80" s="99" t="s">
-        <v>549</v>
-      </c>
-      <c r="D80" s="100">
-        <v>8</v>
-      </c>
-      <c r="E80" s="96" t="s">
-        <v>452</v>
-      </c>
-      <c r="F80" s="101" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="95">
-        <v>7</v>
-      </c>
       <c r="B81" s="99" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C81" s="99" t="s">
         <v>438</v>
@@ -28475,18 +28496,18 @@
         <v>435</v>
       </c>
       <c r="F81" s="101" t="s">
-        <v>500</v>
+        <v>652</v>
       </c>
       <c r="G81" s="56" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="31.5">
       <c r="A82" s="64">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B82" s="99" t="s">
-        <v>502</v>
+        <v>701</v>
       </c>
       <c r="C82" s="99" t="s">
         <v>438</v>
@@ -28498,64 +28519,64 @@
         <v>435</v>
       </c>
       <c r="F82" s="101" t="s">
-        <v>652</v>
+        <v>702</v>
       </c>
       <c r="G82" s="56" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="31.5">
-      <c r="A83" s="64">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="95">
+        <v>9</v>
+      </c>
+      <c r="B83" s="96" t="s">
+        <v>501</v>
+      </c>
+      <c r="C83" s="96" t="s">
+        <v>434</v>
+      </c>
+      <c r="D83" s="97">
         <v>8</v>
-      </c>
-      <c r="B83" s="99" t="s">
-        <v>701</v>
-      </c>
-      <c r="C83" s="99" t="s">
-        <v>438</v>
-      </c>
-      <c r="D83" s="100">
-        <v>2</v>
       </c>
       <c r="E83" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="F83" s="101" t="s">
-        <v>702</v>
+      <c r="F83" s="81" t="s">
+        <v>676</v>
       </c>
       <c r="G83" s="56" t="s">
-        <v>833</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:7">
-      <c r="A84" s="95">
-        <v>9</v>
-      </c>
-      <c r="B84" s="96" t="s">
-        <v>501</v>
-      </c>
-      <c r="C84" s="96" t="s">
-        <v>434</v>
-      </c>
-      <c r="D84" s="97">
+      <c r="A84" s="64">
+        <v>10</v>
+      </c>
+      <c r="B84" s="99" t="s">
+        <v>591</v>
+      </c>
+      <c r="C84" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D84" s="100">
         <v>8</v>
       </c>
       <c r="E84" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="F84" s="81" t="s">
-        <v>676</v>
+      <c r="F84" s="101" t="s">
+        <v>636</v>
       </c>
       <c r="G84" s="56" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:7">
-      <c r="A85" s="64">
-        <v>10</v>
-      </c>
-      <c r="B85" s="99" t="s">
-        <v>591</v>
+      <c r="A85" s="95">
+        <v>11</v>
+      </c>
+      <c r="B85" s="102" t="s">
+        <v>660</v>
       </c>
       <c r="C85" s="99" t="s">
         <v>438</v>
@@ -28566,19 +28587,19 @@
       <c r="E85" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="F85" s="101" t="s">
-        <v>636</v>
+      <c r="F85" s="79" t="s">
+        <v>662</v>
       </c>
       <c r="G85" s="56" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="95">
-        <v>11</v>
+      <c r="A86" s="64">
+        <v>12</v>
       </c>
       <c r="B86" s="102" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C86" s="99" t="s">
         <v>438</v>
@@ -28590,95 +28611,90 @@
         <v>435</v>
       </c>
       <c r="F86" s="79" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="G86" s="56" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="64">
-        <v>12</v>
-      </c>
-      <c r="B87" s="102" t="s">
-        <v>661</v>
-      </c>
-      <c r="C87" s="99" t="s">
-        <v>438</v>
-      </c>
-      <c r="D87" s="100">
-        <v>8</v>
-      </c>
+      <c r="A87" s="95">
+        <v>13</v>
+      </c>
+      <c r="B87" s="96" t="s">
+        <v>640</v>
+      </c>
+      <c r="C87" s="96" t="s">
+        <v>572</v>
+      </c>
+      <c r="D87" s="97"/>
       <c r="E87" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="F87" s="79" t="s">
-        <v>663</v>
+      <c r="F87" s="78" t="s">
+        <v>641</v>
       </c>
       <c r="G87" s="56" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="95">
-        <v>13</v>
+    <row r="88" spans="1:7" ht="31.5">
+      <c r="A88" s="64">
+        <v>14</v>
       </c>
       <c r="B88" s="96" t="s">
-        <v>640</v>
+        <v>648</v>
       </c>
       <c r="C88" s="96" t="s">
-        <v>572</v>
-      </c>
-      <c r="D88" s="97"/>
+        <v>434</v>
+      </c>
+      <c r="D88" s="97">
+        <v>8</v>
+      </c>
       <c r="E88" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="F88" s="78" t="s">
-        <v>641</v>
+      <c r="F88" s="79" t="s">
+        <v>649</v>
       </c>
       <c r="G88" s="56" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="31.5">
-      <c r="A89" s="64">
-        <v>14</v>
+    <row r="89" spans="1:7">
+      <c r="A89" s="95">
+        <v>15</v>
       </c>
       <c r="B89" s="96" t="s">
-        <v>648</v>
+        <v>518</v>
       </c>
       <c r="C89" s="96" t="s">
-        <v>434</v>
-      </c>
-      <c r="D89" s="97">
-        <v>8</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="D89" s="97"/>
       <c r="E89" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="F89" s="79" t="s">
-        <v>649</v>
-      </c>
-      <c r="G89" s="56" t="s">
-        <v>2</v>
+      <c r="F89" s="78" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="90" spans="1:7">
-      <c r="A90" s="95">
-        <v>15</v>
+      <c r="A90" s="64">
+        <v>16</v>
       </c>
       <c r="B90" s="96" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C90" s="96" t="s">
         <v>436</v>
       </c>
       <c r="D90" s="97"/>
       <c r="E90" s="96" t="s">
-        <v>435</v>
+        <v>452</v>
       </c>
       <c r="F90" s="78" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -28709,7 +28725,7 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="104" t="s">
-        <v>726</v>
+        <v>834</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -28757,7 +28773,7 @@
         <v>2</v>
       </c>
       <c r="B97" s="102" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C97" s="96" t="s">
         <v>434</v>
@@ -28893,7 +28909,7 @@
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="104" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -28961,7 +28977,7 @@
         <v>3</v>
       </c>
       <c r="B110" s="102" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C110" s="102" t="s">
         <v>434</v>
@@ -28981,7 +28997,7 @@
         <v>4</v>
       </c>
       <c r="B111" s="102" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C111" s="102" t="s">
         <v>434</v>
@@ -29110,7 +29126,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="96" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C120" s="96" t="s">
         <v>434</v>
@@ -29298,7 +29314,7 @@
         <v>2</v>
       </c>
       <c r="B132" s="96" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C132" s="96" t="s">
         <v>434</v>
@@ -29510,7 +29526,7 @@
         <v>435</v>
       </c>
       <c r="F142" s="101" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -29556,7 +29572,7 @@
     </row>
     <row r="147" spans="1:7" s="11" customFormat="1">
       <c r="A147" s="104" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D147" s="105"/>
       <c r="F147" s="106"/>
@@ -29601,7 +29617,7 @@
         <v>527</v>
       </c>
       <c r="G149" s="56" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -29609,7 +29625,7 @@
         <v>2</v>
       </c>
       <c r="B150" s="96" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C150" s="96" t="s">
         <v>434</v>
@@ -29649,7 +29665,7 @@
         <v>4</v>
       </c>
       <c r="B152" s="96" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="C152" s="96" t="s">
         <v>434</v>
@@ -29661,7 +29677,7 @@
         <v>435</v>
       </c>
       <c r="F152" s="78" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -29669,7 +29685,7 @@
         <v>5</v>
       </c>
       <c r="B153" s="96" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C153" s="96" t="s">
         <v>434</v>
@@ -29681,7 +29697,7 @@
         <v>435</v>
       </c>
       <c r="F153" s="78" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -29689,7 +29705,7 @@
         <v>6</v>
       </c>
       <c r="B154" s="102" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="C154" s="99" t="s">
         <v>572</v>
@@ -29699,7 +29715,7 @@
         <v>435</v>
       </c>
       <c r="F154" s="78" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -29719,7 +29735,7 @@
         <v>435</v>
       </c>
       <c r="F155" s="78" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -29739,7 +29755,7 @@
         <v>435</v>
       </c>
       <c r="F156" s="79" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -29832,7 +29848,7 @@
         <v>527</v>
       </c>
       <c r="G163" s="56" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -29840,7 +29856,7 @@
         <v>6</v>
       </c>
       <c r="B164" s="96" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C164" s="96" t="s">
         <v>434</v>
@@ -29860,7 +29876,7 @@
         <v>2</v>
       </c>
       <c r="B165" s="102" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C165" s="96" t="s">
         <v>434</v>
@@ -29872,7 +29888,7 @@
         <v>435</v>
       </c>
       <c r="F165" s="79" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -29920,7 +29936,7 @@
         <v>5</v>
       </c>
       <c r="B168" s="96" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C168" s="96" t="s">
         <v>434</v>
@@ -29940,7 +29956,7 @@
         <v>6</v>
       </c>
       <c r="B169" s="102" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C169" s="96" t="s">
         <v>434</v>
@@ -29950,7 +29966,7 @@
         <v>452</v>
       </c>
       <c r="F169" s="79" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -30030,7 +30046,7 @@
         <v>435</v>
       </c>
       <c r="F173" s="78" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -30050,7 +30066,7 @@
         <v>435</v>
       </c>
       <c r="F174" s="79" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -30160,7 +30176,7 @@
         <v>452</v>
       </c>
       <c r="F182" s="78" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -30168,7 +30184,7 @@
         <v>3</v>
       </c>
       <c r="B183" s="102" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="C183" s="96" t="s">
         <v>434</v>
@@ -30180,7 +30196,7 @@
         <v>452</v>
       </c>
       <c r="F183" s="79" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -30188,7 +30204,7 @@
         <v>4</v>
       </c>
       <c r="B184" s="96" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C184" s="96" t="s">
         <v>434</v>
@@ -30228,7 +30244,7 @@
         <v>6</v>
       </c>
       <c r="B186" s="96" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C186" s="96" t="s">
         <v>434</v>
@@ -30288,7 +30304,7 @@
         <v>9</v>
       </c>
       <c r="B189" s="99" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C189" s="99" t="s">
         <v>488</v>
@@ -30300,7 +30316,7 @@
         <v>452</v>
       </c>
       <c r="F189" s="101" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -30308,7 +30324,7 @@
         <v>12</v>
       </c>
       <c r="B190" s="99" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="C190" s="99" t="s">
         <v>488</v>
@@ -30320,7 +30336,7 @@
         <v>435</v>
       </c>
       <c r="F190" s="101" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -30488,7 +30504,7 @@
         <v>19</v>
       </c>
       <c r="B199" s="96" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="C199" s="96" t="s">
         <v>436</v>
@@ -30518,7 +30534,7 @@
         <v>435</v>
       </c>
       <c r="F200" s="78" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -30528,7 +30544,7 @@
     </row>
     <row r="203" spans="1:6" s="11" customFormat="1">
       <c r="A203" s="104" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D203" s="105"/>
       <c r="F203" s="106"/>
@@ -30570,7 +30586,7 @@
         <v>435</v>
       </c>
       <c r="F205" s="78" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -30578,7 +30594,7 @@
         <v>2</v>
       </c>
       <c r="B206" s="96" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C206" s="96" t="s">
         <v>434</v>
@@ -30598,7 +30614,7 @@
         <v>3</v>
       </c>
       <c r="B207" s="96" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C207" s="96" t="s">
         <v>434</v>
@@ -30630,7 +30646,7 @@
         <v>435</v>
       </c>
       <c r="F208" s="78" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -30650,7 +30666,7 @@
         <v>435</v>
       </c>
       <c r="F209" s="101" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="210" spans="1:6">
@@ -30658,7 +30674,7 @@
         <v>6</v>
       </c>
       <c r="B210" s="99" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C210" s="99" t="s">
         <v>488</v>
@@ -30670,7 +30686,7 @@
         <v>435</v>
       </c>
       <c r="F210" s="101" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="211" spans="1:6">
@@ -30768,12 +30784,436 @@
         <v>435</v>
       </c>
       <c r="F215" s="78" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="57" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
+      <c r="A218" s="104" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
+      <c r="A219" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B219" s="53" t="s">
+        <v>429</v>
+      </c>
+      <c r="C219" s="53" t="s">
+        <v>430</v>
+      </c>
+      <c r="D219" s="53" t="s">
+        <v>496</v>
+      </c>
+      <c r="E219" s="54" t="s">
+        <v>431</v>
+      </c>
+      <c r="F219" s="55" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6">
+      <c r="A220" s="95">
+        <v>1</v>
+      </c>
+      <c r="B220" s="96" t="s">
+        <v>432</v>
+      </c>
+      <c r="C220" s="96" t="s">
+        <v>434</v>
+      </c>
+      <c r="D220" s="97">
+        <v>8</v>
+      </c>
+      <c r="E220" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F220" s="78" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
+      <c r="A221" s="64">
+        <v>2</v>
+      </c>
+      <c r="B221" s="102" t="s">
+        <v>827</v>
+      </c>
+      <c r="C221" s="96" t="s">
+        <v>434</v>
+      </c>
+      <c r="D221" s="97">
+        <v>8</v>
+      </c>
+      <c r="E221" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F221" s="78" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222" s="64">
+        <v>2</v>
+      </c>
+      <c r="B222" s="102" t="s">
+        <v>584</v>
+      </c>
+      <c r="C222" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="D222" s="100">
+        <v>200</v>
+      </c>
+      <c r="E222" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="F222" s="79" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" s="64">
+        <v>3</v>
+      </c>
+      <c r="B223" s="102" t="s">
+        <v>585</v>
+      </c>
+      <c r="C223" s="99" t="s">
+        <v>488</v>
+      </c>
+      <c r="D223" s="100">
+        <v>50</v>
+      </c>
+      <c r="E223" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F223" s="79" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224" s="64">
+        <v>4</v>
+      </c>
+      <c r="B224" s="99" t="s">
+        <v>552</v>
+      </c>
+      <c r="C224" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D224" s="100">
+        <v>2</v>
+      </c>
+      <c r="E224" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="F224" s="101" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7">
+      <c r="A225" s="95">
+        <v>5</v>
+      </c>
+      <c r="B225" s="102" t="s">
+        <v>587</v>
+      </c>
+      <c r="C225" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D225" s="100">
+        <v>2</v>
+      </c>
+      <c r="E225" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="F225" s="79" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7">
+      <c r="A226" s="64">
+        <v>6</v>
+      </c>
+      <c r="B226" s="99" t="s">
+        <v>547</v>
+      </c>
+      <c r="C226" s="99" t="s">
+        <v>549</v>
+      </c>
+      <c r="D226" s="100">
+        <v>8</v>
+      </c>
+      <c r="E226" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="F226" s="101" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7">
+      <c r="A227" s="95">
+        <v>7</v>
+      </c>
+      <c r="B227" s="99" t="s">
+        <v>499</v>
+      </c>
+      <c r="C227" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D227" s="100">
+        <v>2</v>
+      </c>
+      <c r="E227" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F227" s="101" t="s">
+        <v>500</v>
+      </c>
+      <c r="G227" s="56" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" ht="31.5">
+      <c r="A228" s="64">
+        <v>6</v>
+      </c>
+      <c r="B228" s="99" t="s">
+        <v>502</v>
+      </c>
+      <c r="C228" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D228" s="100">
+        <v>2</v>
+      </c>
+      <c r="E228" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F228" s="101" t="s">
+        <v>652</v>
+      </c>
+      <c r="G228" s="56" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" ht="31.5">
+      <c r="A229" s="64">
+        <v>8</v>
+      </c>
+      <c r="B229" s="99" t="s">
+        <v>701</v>
+      </c>
+      <c r="C229" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D229" s="100">
+        <v>2</v>
+      </c>
+      <c r="E229" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F229" s="101" t="s">
+        <v>702</v>
+      </c>
+      <c r="G229" s="56" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
+      <c r="A230" s="95">
+        <v>9</v>
+      </c>
+      <c r="B230" s="96" t="s">
+        <v>501</v>
+      </c>
+      <c r="C230" s="96" t="s">
+        <v>434</v>
+      </c>
+      <c r="D230" s="97">
+        <v>8</v>
+      </c>
+      <c r="E230" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F230" s="81" t="s">
+        <v>676</v>
+      </c>
+      <c r="G230" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
+      <c r="A231" s="64">
+        <v>10</v>
+      </c>
+      <c r="B231" s="99" t="s">
+        <v>591</v>
+      </c>
+      <c r="C231" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D231" s="100">
+        <v>8</v>
+      </c>
+      <c r="E231" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F231" s="101" t="s">
+        <v>636</v>
+      </c>
+      <c r="G231" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7">
+      <c r="A232" s="95">
+        <v>11</v>
+      </c>
+      <c r="B232" s="102" t="s">
+        <v>660</v>
+      </c>
+      <c r="C232" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D232" s="100">
+        <v>8</v>
+      </c>
+      <c r="E232" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F232" s="79" t="s">
+        <v>662</v>
+      </c>
+      <c r="G232" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7">
+      <c r="A233" s="64">
+        <v>12</v>
+      </c>
+      <c r="B233" s="102" t="s">
+        <v>661</v>
+      </c>
+      <c r="C233" s="99" t="s">
+        <v>438</v>
+      </c>
+      <c r="D233" s="100">
+        <v>8</v>
+      </c>
+      <c r="E233" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F233" s="79" t="s">
+        <v>663</v>
+      </c>
+      <c r="G233" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7">
+      <c r="A234" s="95">
+        <v>13</v>
+      </c>
+      <c r="B234" s="96" t="s">
+        <v>640</v>
+      </c>
+      <c r="C234" s="96" t="s">
+        <v>572</v>
+      </c>
+      <c r="D234" s="97"/>
+      <c r="E234" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F234" s="78" t="s">
+        <v>641</v>
+      </c>
+      <c r="G234" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" ht="31.5">
+      <c r="A235" s="64">
+        <v>14</v>
+      </c>
+      <c r="B235" s="96" t="s">
+        <v>648</v>
+      </c>
+      <c r="C235" s="96" t="s">
+        <v>434</v>
+      </c>
+      <c r="D235" s="97">
+        <v>8</v>
+      </c>
+      <c r="E235" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F235" s="79" t="s">
+        <v>649</v>
+      </c>
+      <c r="G235" s="56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7">
+      <c r="A236" s="95">
+        <v>15</v>
+      </c>
+      <c r="B236" s="96" t="s">
+        <v>518</v>
+      </c>
+      <c r="C236" s="96" t="s">
+        <v>436</v>
+      </c>
+      <c r="D236" s="97"/>
+      <c r="E236" s="96" t="s">
+        <v>435</v>
+      </c>
+      <c r="F236" s="78" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7">
+      <c r="A237" s="64">
+        <v>16</v>
+      </c>
+      <c r="B237" s="96" t="s">
+        <v>519</v>
+      </c>
+      <c r="C237" s="96" t="s">
+        <v>436</v>
+      </c>
+      <c r="D237" s="97"/>
+      <c r="E237" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="F237" s="78" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7">
+      <c r="A238" s="64">
+        <v>16</v>
+      </c>
+      <c r="B238" s="96" t="s">
+        <v>519</v>
+      </c>
+      <c r="C238" s="96" t="s">
+        <v>436</v>
+      </c>
+      <c r="D238" s="97"/>
+      <c r="E238" s="96" t="s">
+        <v>452</v>
+      </c>
+      <c r="F238" s="78" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sửa phần thông tin
</commit_message>
<xml_diff>
--- a/reque/SMS_Gateway_Requirements_20171115.xlsx
+++ b/reque/SMS_Gateway_Requirements_20171115.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2521" uniqueCount="836">
   <si>
     <t>No.</t>
   </si>
@@ -2697,6 +2697,9 @@
   </si>
   <si>
     <t>TABLE "Manager_Setting"=&gt; không dùng</t>
+  </si>
+  <si>
+    <t>device_code</t>
   </si>
 </sst>
 </file>
@@ -27106,8 +27109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -27343,7 +27346,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="96" t="s">
-        <v>574</v>
+        <v>835</v>
       </c>
       <c r="C15" s="96" t="s">
         <v>434</v>

</xml_diff>